<commit_message>
Refactor QLSV.PY to add multiple score entries and calculate average score; update sinhvien.xlsx
</commit_message>
<xml_diff>
--- a/sinhvien.xlsx
+++ b/sinhvien.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,22 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ĐIỂM</t>
+          <t>ĐIỂM 1</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>ĐIỂM 2</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ĐIỂM 3</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>ĐIỂM TB</t>
         </is>
       </c>
     </row>
@@ -491,16 +506,33 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>DH25PM</t>
+          <t>DH25T</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CNTT</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>7</v>
+          <t>Ngoại ngữ</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>6.67</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -521,7 +553,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -531,112 +563,163 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>DH25PM</t>
+          <t>DH25TH</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CNTT</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
+          <t>Sư phạm</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>6.33</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DPM245446</t>
+          <t>DPM245448</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HUYNH PHUC</t>
+          <t>CAO THI TRUC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LAM</t>
+          <t>LINH</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>2006-07-24</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>DH25T</t>
+          <t>DH25PM</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Kinh tế</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>6</v>
+          <t>CNTT</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DPM245448</t>
+          <t>DPM245451</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CAO THI TRUC</t>
+          <t>PHAN THANH</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LINH</t>
+          <t>LOI</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DH25PM</t>
+          <t>DH24PM</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CNTT</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>8</v>
+          <t>Nông nghiệp</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>6.33</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DPM245451</t>
+          <t>DPM245588</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PHAN THANH</t>
+          <t>NGUYEN VAN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LOI</t>
+          <t>AN</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -646,12 +729,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DH25TH</t>
+          <t>DH25PM</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -659,48 +742,25 @@
           <t>CNTT</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>DPM245465</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LAM HUYNH PHUONG</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>LAM</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2000-01-01</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>DH25PM</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>CNTT</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>5</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor QLSV.PY to enhance the save score functionality, update the main table after saving, and automatically close the dialog.
</commit_message>
<xml_diff>
--- a/sinhvien.xlsx
+++ b/sinhvien.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,12 +506,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>DH25T</t>
+          <t>DH25PM</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ngoại ngữ</t>
+          <t>CNTT</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -521,17 +521,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>6.67</t>
+          <t>7.67</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -563,126 +563,126 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>DH25TH</t>
+          <t>DH25T</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Sư phạm</t>
+          <t>Nông nghiệp</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>6.33</t>
+          <t>7.67</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DPM245448</t>
+          <t>DPM245446</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CAO THI TRUC</t>
+          <t>HUYNH PHUC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LINH</t>
+          <t>LAM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2006-07-24</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>DH25PM</t>
+          <t>DH25TH</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CNTT</t>
+          <t>Nông nghiệp</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>7.0</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>8.0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>6.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DPM245451</t>
+          <t>DPM245448</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PHAN THANH</t>
+          <t>CAO THI TRUC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LOI</t>
+          <t>LINH</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DH24PM</t>
+          <t>DH25T</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Nông nghiệp</t>
+          <t>Kinh tế</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -702,24 +702,24 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>6.33</t>
+          <t>8.33</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DPM245588</t>
+          <t>DPM245451</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NGUYEN VAN</t>
+          <t>PHAN THANH</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AN</t>
+          <t>LOI</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -744,22 +744,79 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>5.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DPM245465</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LAM HUYNH PHUONG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LAM</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Nữ</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>DH24PM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sư phạm</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>7.0</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>10.0</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>7.0</t>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>8.0</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>8.0</t>
         </is>
       </c>
     </row>

</xml_diff>